<commit_message>
common data part done
</commit_message>
<xml_diff>
--- a/workbooks/csgo.xlsx
+++ b/workbooks/csgo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidhi_kumar\Desktop\python-db-task1\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C4A4C5-5D53-4363-9776-D3D38E80459E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727A4C6C-3105-4C96-B837-27B634CDD538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,10 +50,10 @@
     <t>Perfecto</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Flamie</t>
+  </si>
+  <si>
+    <t>North Ame</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -409,15 +409,15 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>29</v>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -468,15 +468,15 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>29</v>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,10 +532,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>29</v>

</xml_diff>